<commit_message>
push all system career functions
</commit_message>
<xml_diff>
--- a/public/simples/الدائرى تمهيدى بنات.xlsx
+++ b/public/simples/الدائرى تمهيدى بنات.xlsx
@@ -1,33 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\work\charity\SLS System\تمهيدى - 2024-2025\Ald2ry\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohamed Elsayed\Desktop\sidigaberAdmin\public\simples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A86FCF6A-C202-4844-A781-DA6373F671D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2827CEEE-5DA1-45ED-A1DE-D349A1FA822E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="624" windowWidth="14544" windowHeight="12336" xr2:uid="{57AC980A-7F51-4789-AF6B-F3EFE678C2EE}"/>
+    <workbookView xWindow="3330" yWindow="0" windowWidth="17160" windowHeight="10920" xr2:uid="{57AC980A-7F51-4789-AF6B-F3EFE678C2EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -153,9 +144,6 @@
     <t>دانيا مازن عبد الرحمن ابو العنين  بدر</t>
   </si>
   <si>
-    <t>رنا أشرف محمد ناظن</t>
-  </si>
-  <si>
     <t>روضة محمد عباس إبراهيم</t>
   </si>
   <si>
@@ -331,6 +319,9 @@
   </si>
   <si>
     <t>female</t>
+  </si>
+  <si>
+    <t>رنا أشرف محمد ناظم</t>
   </si>
 </sst>
 </file>
@@ -728,17 +719,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7835FAE8-C31D-4534-9A1F-DE56C901F3DC}">
   <dimension ref="A1:I88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F88"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -767,7 +759,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>32105010200782</v>
       </c>
@@ -775,7 +767,7 @@
         <v>11</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -796,7 +788,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>32104140201962</v>
       </c>
@@ -804,7 +796,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -825,7 +817,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>32010040202568</v>
       </c>
@@ -833,7 +825,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -854,7 +846,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>32107290202869</v>
       </c>
@@ -862,7 +854,7 @@
         <v>14</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -883,7 +875,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>32108080201343</v>
       </c>
@@ -891,7 +883,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -912,7 +904,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>32010011822409</v>
       </c>
@@ -920,7 +912,7 @@
         <v>16</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -941,7 +933,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>32101110201225</v>
       </c>
@@ -949,7 +941,7 @@
         <v>17</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -970,7 +962,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>32010030200621</v>
       </c>
@@ -978,7 +970,7 @@
         <v>18</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -999,7 +991,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>32010040202541</v>
       </c>
@@ -1007,7 +999,7 @@
         <v>19</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -1028,7 +1020,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>32010220201721</v>
       </c>
@@ -1036,7 +1028,7 @@
         <v>20</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -1057,7 +1049,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>32109170200903</v>
       </c>
@@ -1065,7 +1057,7 @@
         <v>21</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -1086,7 +1078,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>32011170200563</v>
       </c>
@@ -1094,7 +1086,7 @@
         <v>22</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -1115,7 +1107,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>32105150200243</v>
       </c>
@@ -1123,7 +1115,7 @@
         <v>23</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -1144,7 +1136,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>32106080200549</v>
       </c>
@@ -1152,7 +1144,7 @@
         <v>24</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -1173,7 +1165,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>32103170201383</v>
       </c>
@@ -1181,7 +1173,7 @@
         <v>25</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -1202,7 +1194,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>32105230200325</v>
       </c>
@@ -1210,7 +1202,7 @@
         <v>26</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -1231,7 +1223,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>32107060201944</v>
       </c>
@@ -1239,7 +1231,7 @@
         <v>27</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -1260,7 +1252,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>32107170202105</v>
       </c>
@@ -1268,7 +1260,7 @@
         <v>28</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -1289,7 +1281,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>32102260200665</v>
       </c>
@@ -1297,7 +1289,7 @@
         <v>29</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -1318,7 +1310,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>32101090200707</v>
       </c>
@@ -1326,7 +1318,7 @@
         <v>30</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -1347,7 +1339,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>32010100201167</v>
       </c>
@@ -1355,7 +1347,7 @@
         <v>31</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -1376,7 +1368,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>32102040200184</v>
       </c>
@@ -1384,7 +1376,7 @@
         <v>32</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -1405,7 +1397,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>32103210201586</v>
       </c>
@@ -1413,7 +1405,7 @@
         <v>33</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -1434,7 +1426,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>32011030200768</v>
       </c>
@@ -1442,7 +1434,7 @@
         <v>34</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -1463,7 +1455,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>32101260200049</v>
       </c>
@@ -1471,7 +1463,7 @@
         <v>35</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -1492,7 +1484,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>32104110200368</v>
       </c>
@@ -1500,7 +1492,7 @@
         <v>36</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -1521,7 +1513,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>32101170200503</v>
       </c>
@@ -1529,7 +1521,7 @@
         <v>37</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -1550,7 +1542,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>32010130201226</v>
       </c>
@@ -1558,7 +1550,7 @@
         <v>38</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -1579,15 +1571,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>32103250201465</v>
       </c>
       <c r="B30" t="s">
-        <v>39</v>
+        <v>98</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -1608,15 +1600,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>32010150202563</v>
       </c>
       <c r="B31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D31">
         <v>1</v>
@@ -1637,15 +1629,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>32010040201049</v>
       </c>
       <c r="B32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -1666,15 +1658,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>32106260201268</v>
       </c>
       <c r="B33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -1695,15 +1687,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>32102010200368</v>
       </c>
       <c r="B34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -1724,15 +1716,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>32107300201149</v>
       </c>
       <c r="B35" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D35">
         <v>1</v>
@@ -1753,15 +1745,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>32011200201349</v>
       </c>
       <c r="B36" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D36">
         <v>1</v>
@@ -1782,15 +1774,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>32103080201481</v>
       </c>
       <c r="B37" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -1811,15 +1803,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>32105270202584</v>
       </c>
       <c r="B38" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -1840,15 +1832,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>32010200204104</v>
       </c>
       <c r="B39" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D39">
         <v>1</v>
@@ -1869,15 +1861,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>32103280201222</v>
       </c>
       <c r="B40" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D40">
         <v>1</v>
@@ -1898,15 +1890,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>32101270201027</v>
       </c>
       <c r="B41" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D41">
         <v>1</v>
@@ -1927,15 +1919,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>32102100203382</v>
       </c>
       <c r="B42" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D42">
         <v>1</v>
@@ -1956,15 +1948,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>32011010203787</v>
       </c>
       <c r="B43" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -1985,15 +1977,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>32011190201485</v>
       </c>
       <c r="B44" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D44">
         <v>1</v>
@@ -2014,15 +2006,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>32103060200764</v>
       </c>
       <c r="B45" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D45">
         <v>1</v>
@@ -2043,15 +2035,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>32104280201067</v>
       </c>
       <c r="B46" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D46">
         <v>1</v>
@@ -2072,15 +2064,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>32012170202562</v>
       </c>
       <c r="B47" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D47">
         <v>1</v>
@@ -2101,15 +2093,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>32105200200703</v>
       </c>
       <c r="B48" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D48">
         <v>1</v>
@@ -2130,15 +2122,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>32109140200542</v>
       </c>
       <c r="B49" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D49">
         <v>1</v>
@@ -2159,15 +2151,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>32011280202286</v>
       </c>
       <c r="B50" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D50">
         <v>1</v>
@@ -2188,15 +2180,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>32010250201807</v>
       </c>
       <c r="B51" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D51">
         <v>1</v>
@@ -2217,15 +2209,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>32109110200181</v>
       </c>
       <c r="B52" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D52">
         <v>1</v>
@@ -2246,15 +2238,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>32104150201588</v>
       </c>
       <c r="B53" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D53">
         <v>1</v>
@@ -2275,15 +2267,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>32103210200504</v>
       </c>
       <c r="B54" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D54">
         <v>1</v>
@@ -2304,15 +2296,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>32012090201727</v>
       </c>
       <c r="B55" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D55">
         <v>1</v>
@@ -2333,15 +2325,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>32010190201845</v>
       </c>
       <c r="B56" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D56">
         <v>1</v>
@@ -2362,15 +2354,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>32012120201603</v>
       </c>
       <c r="B57" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D57">
         <v>1</v>
@@ -2391,15 +2383,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>32012260201921</v>
       </c>
       <c r="B58" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D58">
         <v>1</v>
@@ -2420,15 +2412,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>32102240201142</v>
       </c>
       <c r="B59" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D59">
         <v>1</v>
@@ -2449,15 +2441,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>32012280201928</v>
       </c>
       <c r="B60" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D60">
         <v>1</v>
@@ -2478,15 +2470,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>32103100202447</v>
       </c>
       <c r="B61" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D61">
         <v>1</v>
@@ -2507,15 +2499,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>32012170200543</v>
       </c>
       <c r="B62" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D62">
         <v>1</v>
@@ -2536,15 +2528,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>32106170202567</v>
       </c>
       <c r="B63" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D63">
         <v>1</v>
@@ -2565,15 +2557,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>32010110202706</v>
       </c>
       <c r="B64" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D64">
         <v>1</v>
@@ -2594,15 +2586,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>32010120200264</v>
       </c>
       <c r="B65" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D65">
         <v>1</v>
@@ -2623,15 +2615,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>32109250203288</v>
       </c>
       <c r="B66" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D66">
         <v>1</v>
@@ -2652,15 +2644,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>32103130200961</v>
       </c>
       <c r="B67" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D67">
         <v>1</v>
@@ -2681,15 +2673,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>32010100205227</v>
       </c>
       <c r="B68" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D68">
         <v>1</v>
@@ -2710,15 +2702,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>32107040202103</v>
       </c>
       <c r="B69" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D69">
         <v>1</v>
@@ -2739,15 +2731,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>32108250202501</v>
       </c>
       <c r="B70" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D70">
         <v>1</v>
@@ -2768,15 +2760,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>32103170201405</v>
       </c>
       <c r="B71" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D71">
         <v>1</v>
@@ -2797,15 +2789,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>32109010201148</v>
       </c>
       <c r="B72" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D72">
         <v>1</v>
@@ -2826,15 +2818,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>32109120200325</v>
       </c>
       <c r="B73" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D73">
         <v>1</v>
@@ -2855,15 +2847,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>32105290200669</v>
       </c>
       <c r="B74" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D74">
         <v>1</v>
@@ -2884,15 +2876,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>32108090202224</v>
       </c>
       <c r="B75" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D75">
         <v>1</v>
@@ -2913,15 +2905,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>32105310200148</v>
       </c>
       <c r="B76" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D76">
         <v>1</v>
@@ -2942,15 +2934,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <v>32106150201408</v>
       </c>
       <c r="B77" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D77">
         <v>1</v>
@@ -2971,15 +2963,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>32012170200861</v>
       </c>
       <c r="B78" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D78">
         <v>1</v>
@@ -3000,15 +2992,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>32101170200406</v>
       </c>
       <c r="B79" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D79">
         <v>1</v>
@@ -3029,15 +3021,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>32106210201186</v>
       </c>
       <c r="B80" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D80">
         <v>1</v>
@@ -3058,15 +3050,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>32107280201163</v>
       </c>
       <c r="B81" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D81">
         <v>1</v>
@@ -3087,15 +3079,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>32108190200709</v>
       </c>
       <c r="B82" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D82">
         <v>1</v>
@@ -3116,15 +3108,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <v>32010140201623</v>
       </c>
       <c r="B83" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D83">
         <v>1</v>
@@ -3145,15 +3137,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>32107150203288</v>
       </c>
       <c r="B84" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D84">
         <v>1</v>
@@ -3174,15 +3166,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>32010160201182</v>
       </c>
       <c r="B85" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D85">
         <v>1</v>
@@ -3203,15 +3195,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
         <v>32104120200781</v>
       </c>
       <c r="B86" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D86">
         <v>1</v>
@@ -3232,15 +3224,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>32010160201166</v>
       </c>
       <c r="B87" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D87">
         <v>1</v>
@@ -3261,15 +3253,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
         <v>32107290201781</v>
       </c>
       <c r="B88" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D88">
         <v>1</v>

</xml_diff>